<commit_message>
Andrew | Added statutes due to (a) needing to collect application requirements, (b) were corrupted, or (c) were not downloaded originally (but cited).
</commit_message>
<xml_diff>
--- a/compliance/Federal Compliance Analysis.xlsx
+++ b/compliance/Federal Compliance Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewhetzler/Documents/Documents - Andrew’s Money Maker/School/DISSERTATION/GitHub/dissertation/compliance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A34D36-2D41-1D4C-ACAB-66A049D0C234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97751D15-A35E-7549-BC8F-CF6A912CF62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="520" windowWidth="40860" windowHeight="24400" firstSheet="3" activeTab="11" xr2:uid="{E5CECD30-7D37-2B4A-8954-83C96D258B13}"/>
+    <workbookView xWindow="-22320" yWindow="500" windowWidth="22320" windowHeight="14620" firstSheet="7" activeTab="11" xr2:uid="{E5CECD30-7D37-2B4A-8954-83C96D258B13}"/>
   </bookViews>
   <sheets>
     <sheet name="FMVSS Certification" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,9 @@
     <sheet name="Recalls - Info - 573.15" sheetId="12" r:id="rId11"/>
     <sheet name="Recalls - Bankruptcy - 573.16" sheetId="14" r:id="rId12"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FMVSS Certification'!$A$1:$A$53</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -999,7 +1002,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1018,6 +1021,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1356,23 +1362,23 @@
   <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.1640625" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="2" max="2" width="20" style="4" customWidth="1"/>
     <col min="3" max="3" width="42.1640625" customWidth="1"/>
     <col min="4" max="4" width="31.83203125" customWidth="1"/>
     <col min="5" max="5" width="86.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1385,11 +1391,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
@@ -1402,11 +1408,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
@@ -1419,11 +1425,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
@@ -1436,11 +1442,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="s">
@@ -1453,11 +1459,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C6" t="s">
@@ -1470,11 +1476,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C7" t="s">
@@ -1487,11 +1493,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C8" t="s">
@@ -1504,11 +1510,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C9" t="s">
@@ -1518,11 +1524,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C10" t="s">
@@ -1535,11 +1541,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C11" t="s">
@@ -1552,11 +1558,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C12" t="s">
@@ -1566,11 +1572,11 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C14" t="s">
@@ -1583,11 +1589,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C15" t="s">
@@ -1600,11 +1606,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C16" t="s">
@@ -1614,11 +1620,11 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C17" t="s">
@@ -1631,11 +1637,11 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>35</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C19" t="s">
@@ -1648,11 +1654,11 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>35</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C20" t="s">
@@ -1665,11 +1671,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>35</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C21" t="s">
@@ -1682,11 +1688,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>35</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C22" t="s">
@@ -1699,11 +1705,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>35</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C23" t="s">
@@ -1716,11 +1722,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>35</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C24" t="s">
@@ -1730,11 +1736,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>39</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C25" t="s">
@@ -1747,11 +1753,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>39</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C26" t="s">
@@ -1764,11 +1770,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>39</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C27" t="s">
@@ -1781,11 +1787,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>39</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C28" t="s">
@@ -1798,11 +1804,11 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>39</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C29" t="s">
@@ -1815,11 +1821,11 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>39</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C30" t="s">
@@ -1829,11 +1835,11 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>42</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C31" t="s">
@@ -1846,11 +1852,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>42</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C32" t="s">
@@ -1863,11 +1869,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>42</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C33" t="s">
@@ -1880,11 +1886,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>42</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C34" t="s">
@@ -1897,11 +1903,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>42</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C35" t="s">
@@ -1914,11 +1920,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>42</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C36" t="s">
@@ -1931,11 +1937,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>42</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C37" t="s">
@@ -1945,11 +1951,11 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>42</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C38" t="s">
@@ -1959,11 +1965,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>42</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C39" t="s">
@@ -1973,11 +1979,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>46</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C41" t="s">
@@ -1987,11 +1993,11 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>46</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C42" t="s">
@@ -2004,11 +2010,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>46</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C43" t="s">
@@ -2021,11 +2027,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>46</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C44" t="s">
@@ -2038,11 +2044,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>48</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C46" t="s">
@@ -2055,11 +2061,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>48</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C47" t="s">
@@ -2072,11 +2078,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>48</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C48" t="s">
@@ -2089,11 +2095,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C49" t="s">
@@ -2106,11 +2112,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C50" t="s">
@@ -2123,11 +2129,11 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>48</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="4" t="s">
         <v>50</v>
       </c>
       <c r="C51" t="s">
@@ -2137,11 +2143,11 @@
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>48</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C52" t="s">
@@ -2154,11 +2160,11 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>48</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C53" t="s">
@@ -2169,6 +2175,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A53" xr:uid="{2FB94E3D-C5C3-3841-8945-149F56AC5305}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2617,7 +2624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB91F4C-9B39-3A40-8192-21E9418B0B76}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:D5"/>
     </sheetView>
   </sheetViews>
@@ -3298,7 +3305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A11599B-9DA0-2045-BC7A-DB9B12AD7FC4}">
   <dimension ref="A2:H316"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -4449,7 +4456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A0ADB2-F801-754C-A5FB-AE093201071A}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -4875,7 +4882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD18739-0A8F-2D47-A6B3-6B11335B6D41}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Andrew | Saved changes to excel spreadsheets. Deleted the temporary spreadsheets.
</commit_message>
<xml_diff>
--- a/compliance/Federal Compliance Analysis.xlsx
+++ b/compliance/Federal Compliance Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewhetzler/Documents/Documents - Andrew’s Money Maker/School/DISSERTATION/GitHub/dissertation/compliance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97751D15-A35E-7549-BC8F-CF6A912CF62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DEE3589-F6AE-1C4C-BF13-C3823E73C126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22320" yWindow="500" windowWidth="22320" windowHeight="14620" firstSheet="7" activeTab="11" xr2:uid="{E5CECD30-7D37-2B4A-8954-83C96D258B13}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22320" windowHeight="14620" xr2:uid="{E5CECD30-7D37-2B4A-8954-83C96D258B13}"/>
   </bookViews>
   <sheets>
     <sheet name="FMVSS Certification" sheetId="1" r:id="rId1"/>
@@ -1359,10 +1359,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB94E3D-C5C3-3841-8945-149F56AC5305}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1391,7 +1392,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1408,7 +1409,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1425,7 +1426,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1442,7 +1443,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1459,7 +1460,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1476,7 +1477,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1493,7 +1494,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1510,7 +1511,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1524,7 +1525,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1541,7 +1542,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1558,7 +1559,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1572,7 +1573,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1589,7 +1591,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1606,7 +1608,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1620,7 +1622,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1637,7 +1639,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1654,7 +1657,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1671,7 +1674,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1688,7 +1691,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -1705,7 +1708,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -1722,7 +1725,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1736,7 +1739,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1753,7 +1756,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1770,7 +1773,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1787,7 +1790,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1804,7 +1807,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1821,7 +1824,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -1835,7 +1838,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -1852,7 +1855,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1869,7 +1872,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -1886,7 +1889,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1903,7 +1906,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -1920,7 +1923,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1937,7 +1940,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -1951,7 +1954,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -1965,7 +1968,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1979,7 +1982,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -1993,7 +1997,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -2010,7 +2014,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -2027,7 +2031,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -2044,6 +2048,7 @@
         <v>1</v>
       </c>
     </row>
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>48</v>
@@ -2175,7 +2180,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A53" xr:uid="{2FB94E3D-C5C3-3841-8945-149F56AC5305}"/>
+  <autoFilter ref="A1:A53" xr:uid="{2FB94E3D-C5C3-3841-8945-149F56AC5305}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Replica Vehicle Manufacturers"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3020,7 +3031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F0D4F19-26C0-D54A-A350-1581CF924F5D}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>